<commit_message>
files with time stamp
</commit_message>
<xml_diff>
--- a/SurveyResults.xlsx
+++ b/SurveyResults.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10116"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10312"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jiayueliu/Desktop/BME580/stress/Stress-Detection-in-Nurses-main/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jiayueliu/Desktop/BME580/BME580/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BB609AD-D820-E64E-BD70-70EBA1473073}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF340D0C-4CB5-3B4F-9366-AE1AD10A218E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2400" yWindow="1420" windowWidth="37340" windowHeight="17860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1140" yWindow="1420" windowWidth="37260" windowHeight="17860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="in" sheetId="1" r:id="rId1"/>
@@ -1361,7 +1361,6 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:T885"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
@@ -1455,7 +1454,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="2" spans="1:20" hidden="1">
+    <row r="2" spans="1:20">
       <c r="A2" s="1" t="s">
         <v>143</v>
       </c>
@@ -1517,7 +1516,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="3" spans="1:20" hidden="1">
+    <row r="3" spans="1:20">
       <c r="A3" s="1" t="s">
         <v>143</v>
       </c>
@@ -1579,7 +1578,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="4" spans="1:20" hidden="1">
+    <row r="4" spans="1:20">
       <c r="A4" s="1" t="s">
         <v>145</v>
       </c>
@@ -1641,7 +1640,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:20" hidden="1">
+    <row r="5" spans="1:20">
       <c r="A5" s="1" t="s">
         <v>145</v>
       </c>
@@ -1765,7 +1764,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="7" spans="1:20" hidden="1">
+    <row r="7" spans="1:20">
       <c r="A7" s="1">
         <v>94</v>
       </c>
@@ -1827,7 +1826,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="8" spans="1:20" hidden="1">
+    <row r="8" spans="1:20">
       <c r="A8" s="1">
         <v>94</v>
       </c>
@@ -1889,7 +1888,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="9" spans="1:20" hidden="1">
+    <row r="9" spans="1:20">
       <c r="A9" s="1" t="s">
         <v>145</v>
       </c>
@@ -1951,7 +1950,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="10" spans="1:20" hidden="1">
+    <row r="10" spans="1:20">
       <c r="A10" s="1" t="s">
         <v>145</v>
       </c>
@@ -2137,7 +2136,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="13" spans="1:20" hidden="1">
+    <row r="13" spans="1:20">
       <c r="A13" s="1" t="s">
         <v>145</v>
       </c>
@@ -2199,7 +2198,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="14" spans="1:20" hidden="1">
+    <row r="14" spans="1:20">
       <c r="A14" s="1" t="s">
         <v>145</v>
       </c>
@@ -2261,7 +2260,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="15" spans="1:20" hidden="1">
+    <row r="15" spans="1:20">
       <c r="A15" s="1" t="s">
         <v>145</v>
       </c>
@@ -2323,7 +2322,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="16" spans="1:20" hidden="1">
+    <row r="16" spans="1:20">
       <c r="A16" s="1" t="s">
         <v>145</v>
       </c>
@@ -2385,7 +2384,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="17" spans="1:20" hidden="1">
+    <row r="17" spans="1:20">
       <c r="A17" s="1" t="s">
         <v>145</v>
       </c>
@@ -2447,7 +2446,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="18" spans="1:20" hidden="1">
+    <row r="18" spans="1:20">
       <c r="A18" s="1">
         <v>94</v>
       </c>
@@ -2509,7 +2508,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="19" spans="1:20" hidden="1">
+    <row r="19" spans="1:20">
       <c r="A19" s="1" t="s">
         <v>145</v>
       </c>
@@ -2571,7 +2570,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="20" spans="1:20" hidden="1">
+    <row r="20" spans="1:20">
       <c r="A20" s="1" t="s">
         <v>145</v>
       </c>
@@ -2633,7 +2632,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="21" spans="1:20" hidden="1">
+    <row r="21" spans="1:20">
       <c r="A21" s="1" t="s">
         <v>145</v>
       </c>
@@ -3129,7 +3128,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="29" spans="1:20" hidden="1">
+    <row r="29" spans="1:20">
       <c r="A29" s="1">
         <v>94</v>
       </c>
@@ -3191,7 +3190,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="30" spans="1:20" hidden="1">
+    <row r="30" spans="1:20">
       <c r="A30" s="1">
         <v>94</v>
       </c>
@@ -3253,7 +3252,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="31" spans="1:20" hidden="1">
+    <row r="31" spans="1:20">
       <c r="A31" s="1">
         <v>94</v>
       </c>
@@ -3315,7 +3314,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="32" spans="1:20" hidden="1">
+    <row r="32" spans="1:20">
       <c r="A32" s="1">
         <v>94</v>
       </c>
@@ -3377,7 +3376,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="33" spans="1:20" hidden="1">
+    <row r="33" spans="1:20">
       <c r="A33" s="1" t="s">
         <v>145</v>
       </c>
@@ -3439,7 +3438,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="34" spans="1:20" hidden="1">
+    <row r="34" spans="1:20">
       <c r="A34" s="1" t="s">
         <v>145</v>
       </c>
@@ -3501,7 +3500,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="35" spans="1:20" hidden="1">
+    <row r="35" spans="1:20">
       <c r="A35" s="1" t="s">
         <v>147</v>
       </c>
@@ -3563,7 +3562,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="36" spans="1:20" hidden="1">
+    <row r="36" spans="1:20">
       <c r="A36" s="1" t="s">
         <v>147</v>
       </c>
@@ -3625,7 +3624,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="37" spans="1:20" hidden="1">
+    <row r="37" spans="1:20">
       <c r="A37" s="1" t="s">
         <v>147</v>
       </c>
@@ -3687,7 +3686,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="38" spans="1:20" hidden="1">
+    <row r="38" spans="1:20">
       <c r="A38" s="1" t="s">
         <v>147</v>
       </c>
@@ -3749,7 +3748,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="39" spans="1:20" hidden="1">
+    <row r="39" spans="1:20">
       <c r="A39" s="1" t="s">
         <v>145</v>
       </c>
@@ -3935,7 +3934,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="42" spans="1:20" hidden="1">
+    <row r="42" spans="1:20">
       <c r="A42" s="1" t="s">
         <v>143</v>
       </c>
@@ -3997,7 +3996,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="43" spans="1:20" hidden="1">
+    <row r="43" spans="1:20">
       <c r="A43" s="1" t="s">
         <v>147</v>
       </c>
@@ -4059,7 +4058,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="44" spans="1:20" hidden="1">
+    <row r="44" spans="1:20">
       <c r="A44" s="1" t="s">
         <v>149</v>
       </c>
@@ -4121,7 +4120,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="45" spans="1:20" hidden="1">
+    <row r="45" spans="1:20">
       <c r="A45" s="1" t="s">
         <v>149</v>
       </c>
@@ -4183,7 +4182,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="46" spans="1:20" hidden="1">
+    <row r="46" spans="1:20">
       <c r="A46" s="1" t="s">
         <v>149</v>
       </c>
@@ -4245,7 +4244,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="47" spans="1:20" hidden="1">
+    <row r="47" spans="1:20">
       <c r="A47" s="1" t="s">
         <v>149</v>
       </c>
@@ -4307,7 +4306,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="48" spans="1:20" hidden="1">
+    <row r="48" spans="1:20">
       <c r="A48" s="1" t="s">
         <v>18</v>
       </c>
@@ -4369,7 +4368,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="49" spans="1:20" hidden="1">
+    <row r="49" spans="1:20">
       <c r="A49" s="1" t="s">
         <v>143</v>
       </c>
@@ -4431,7 +4430,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="50" spans="1:20" hidden="1">
+    <row r="50" spans="1:20">
       <c r="A50" s="1" t="s">
         <v>143</v>
       </c>
@@ -4493,7 +4492,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="51" spans="1:20" hidden="1">
+    <row r="51" spans="1:20">
       <c r="A51" s="1" t="s">
         <v>143</v>
       </c>
@@ -4555,7 +4554,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="52" spans="1:20" hidden="1">
+    <row r="52" spans="1:20">
       <c r="A52" s="1" t="s">
         <v>149</v>
       </c>
@@ -4617,7 +4616,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="53" spans="1:20" hidden="1">
+    <row r="53" spans="1:20">
       <c r="A53" s="1" t="s">
         <v>149</v>
       </c>
@@ -4803,7 +4802,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="56" spans="1:20" hidden="1">
+    <row r="56" spans="1:20">
       <c r="A56" s="1">
         <v>94</v>
       </c>
@@ -4927,7 +4926,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="58" spans="1:20" hidden="1">
+    <row r="58" spans="1:20">
       <c r="A58" s="1">
         <v>94</v>
       </c>
@@ -4989,7 +4988,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="59" spans="1:20" hidden="1">
+    <row r="59" spans="1:20">
       <c r="A59" s="1" t="s">
         <v>143</v>
       </c>
@@ -5051,7 +5050,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="60" spans="1:20" hidden="1">
+    <row r="60" spans="1:20">
       <c r="A60" s="1" t="s">
         <v>143</v>
       </c>
@@ -5113,7 +5112,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="61" spans="1:20" hidden="1">
+    <row r="61" spans="1:20">
       <c r="A61" s="1" t="s">
         <v>149</v>
       </c>
@@ -5175,7 +5174,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="62" spans="1:20" hidden="1">
+    <row r="62" spans="1:20">
       <c r="A62" s="1" t="s">
         <v>149</v>
       </c>
@@ -5237,7 +5236,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="63" spans="1:20" hidden="1">
+    <row r="63" spans="1:20">
       <c r="A63" s="1" t="s">
         <v>147</v>
       </c>
@@ -5299,7 +5298,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="64" spans="1:20" hidden="1">
+    <row r="64" spans="1:20">
       <c r="A64" s="1" t="s">
         <v>147</v>
       </c>
@@ -5361,7 +5360,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="65" spans="1:20" hidden="1">
+    <row r="65" spans="1:20">
       <c r="A65" s="1" t="s">
         <v>143</v>
       </c>
@@ -5423,7 +5422,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="66" spans="1:20" hidden="1">
+    <row r="66" spans="1:20">
       <c r="A66" s="1" t="s">
         <v>143</v>
       </c>
@@ -5485,7 +5484,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="67" spans="1:20" hidden="1">
+    <row r="67" spans="1:20">
       <c r="A67" s="1" t="s">
         <v>145</v>
       </c>
@@ -5547,7 +5546,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="68" spans="1:20" hidden="1">
+    <row r="68" spans="1:20">
       <c r="A68" s="1" t="s">
         <v>143</v>
       </c>
@@ -5609,7 +5608,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="69" spans="1:20" hidden="1">
+    <row r="69" spans="1:20">
       <c r="A69" s="1" t="s">
         <v>143</v>
       </c>
@@ -5671,7 +5670,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="70" spans="1:20" hidden="1">
+    <row r="70" spans="1:20">
       <c r="A70" s="1" t="s">
         <v>143</v>
       </c>
@@ -5733,7 +5732,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="71" spans="1:20" hidden="1">
+    <row r="71" spans="1:20">
       <c r="A71" s="1">
         <v>94</v>
       </c>
@@ -5795,7 +5794,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="72" spans="1:20" hidden="1">
+    <row r="72" spans="1:20">
       <c r="A72" s="1">
         <v>94</v>
       </c>
@@ -5857,7 +5856,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="73" spans="1:20" hidden="1">
+    <row r="73" spans="1:20">
       <c r="A73" s="1" t="s">
         <v>145</v>
       </c>
@@ -6043,7 +6042,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="76" spans="1:20" hidden="1">
+    <row r="76" spans="1:20">
       <c r="A76" s="1" t="s">
         <v>149</v>
       </c>
@@ -6105,7 +6104,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="77" spans="1:20" hidden="1">
+    <row r="77" spans="1:20">
       <c r="A77" s="1" t="s">
         <v>149</v>
       </c>
@@ -6167,7 +6166,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="78" spans="1:20" hidden="1">
+    <row r="78" spans="1:20">
       <c r="A78" s="1" t="s">
         <v>147</v>
       </c>
@@ -6353,7 +6352,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="81" spans="1:20" hidden="1">
+    <row r="81" spans="1:20">
       <c r="A81" s="1" t="s">
         <v>149</v>
       </c>
@@ -6415,7 +6414,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="82" spans="1:20" hidden="1">
+    <row r="82" spans="1:20">
       <c r="A82" s="1">
         <v>94</v>
       </c>
@@ -6477,7 +6476,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="83" spans="1:20" hidden="1">
+    <row r="83" spans="1:20">
       <c r="A83" s="1">
         <v>94</v>
       </c>
@@ -6539,7 +6538,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="84" spans="1:20" hidden="1">
+    <row r="84" spans="1:20">
       <c r="A84" s="1" t="s">
         <v>143</v>
       </c>
@@ -6601,7 +6600,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="85" spans="1:20" hidden="1">
+    <row r="85" spans="1:20">
       <c r="A85" s="1" t="s">
         <v>143</v>
       </c>
@@ -6663,7 +6662,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="86" spans="1:20" hidden="1">
+    <row r="86" spans="1:20">
       <c r="A86" s="1">
         <v>94</v>
       </c>
@@ -6725,7 +6724,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="87" spans="1:20" hidden="1">
+    <row r="87" spans="1:20">
       <c r="A87" s="1">
         <v>94</v>
       </c>
@@ -6849,7 +6848,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="89" spans="1:20" hidden="1">
+    <row r="89" spans="1:20">
       <c r="A89" s="1" t="s">
         <v>149</v>
       </c>
@@ -6911,7 +6910,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="90" spans="1:20" hidden="1">
+    <row r="90" spans="1:20">
       <c r="A90" s="1" t="s">
         <v>147</v>
       </c>
@@ -6973,7 +6972,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="91" spans="1:20" hidden="1">
+    <row r="91" spans="1:20">
       <c r="A91" s="1" t="s">
         <v>147</v>
       </c>
@@ -7035,7 +7034,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="92" spans="1:20" hidden="1">
+    <row r="92" spans="1:20">
       <c r="A92" s="1">
         <v>94</v>
       </c>
@@ -7097,7 +7096,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="93" spans="1:20" hidden="1">
+    <row r="93" spans="1:20">
       <c r="A93" s="1">
         <v>94</v>
       </c>
@@ -7159,7 +7158,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="94" spans="1:20" hidden="1">
+    <row r="94" spans="1:20">
       <c r="A94" s="1" t="s">
         <v>149</v>
       </c>
@@ -7283,7 +7282,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="96" spans="1:20" hidden="1">
+    <row r="96" spans="1:20">
       <c r="A96" s="1">
         <v>94</v>
       </c>
@@ -7345,7 +7344,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="97" spans="1:20" hidden="1">
+    <row r="97" spans="1:20">
       <c r="A97" s="1" t="s">
         <v>145</v>
       </c>
@@ -7407,7 +7406,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="98" spans="1:20" hidden="1">
+    <row r="98" spans="1:20">
       <c r="A98" s="1" t="s">
         <v>145</v>
       </c>
@@ -7469,7 +7468,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="99" spans="1:20" hidden="1">
+    <row r="99" spans="1:20">
       <c r="A99" s="1" t="s">
         <v>145</v>
       </c>
@@ -7531,7 +7530,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="100" spans="1:20" hidden="1">
+    <row r="100" spans="1:20">
       <c r="A100" s="1" t="s">
         <v>149</v>
       </c>
@@ -7593,7 +7592,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="101" spans="1:20" hidden="1">
+    <row r="101" spans="1:20">
       <c r="A101" s="1" t="s">
         <v>149</v>
       </c>
@@ -7655,7 +7654,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="102" spans="1:20" hidden="1">
+    <row r="102" spans="1:20">
       <c r="A102" s="1" t="s">
         <v>149</v>
       </c>
@@ -7717,7 +7716,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="103" spans="1:20" hidden="1">
+    <row r="103" spans="1:20">
       <c r="A103" s="1" t="s">
         <v>149</v>
       </c>
@@ -7779,7 +7778,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="104" spans="1:20" hidden="1">
+    <row r="104" spans="1:20">
       <c r="A104" s="1">
         <v>94</v>
       </c>
@@ -7841,7 +7840,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="105" spans="1:20" hidden="1">
+    <row r="105" spans="1:20">
       <c r="A105" s="1">
         <v>94</v>
       </c>
@@ -7903,7 +7902,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="106" spans="1:20" hidden="1">
+    <row r="106" spans="1:20">
       <c r="A106" s="1" t="s">
         <v>147</v>
       </c>
@@ -7965,7 +7964,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="107" spans="1:20" hidden="1">
+    <row r="107" spans="1:20">
       <c r="A107" s="1" t="s">
         <v>147</v>
       </c>
@@ -8027,7 +8026,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="108" spans="1:20" hidden="1">
+    <row r="108" spans="1:20">
       <c r="A108" s="1" t="s">
         <v>147</v>
       </c>
@@ -8337,7 +8336,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="113" spans="1:20" hidden="1">
+    <row r="113" spans="1:20">
       <c r="A113" s="1" t="s">
         <v>149</v>
       </c>
@@ -8399,7 +8398,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="114" spans="1:20" hidden="1">
+    <row r="114" spans="1:20">
       <c r="A114" s="1">
         <v>94</v>
       </c>
@@ -8461,7 +8460,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="115" spans="1:20" hidden="1">
+    <row r="115" spans="1:20">
       <c r="A115" s="1">
         <v>94</v>
       </c>
@@ -8523,7 +8522,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="116" spans="1:20" hidden="1">
+    <row r="116" spans="1:20">
       <c r="A116" s="1" t="s">
         <v>149</v>
       </c>
@@ -8585,7 +8584,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="117" spans="1:20" hidden="1">
+    <row r="117" spans="1:20">
       <c r="A117" s="1" t="s">
         <v>147</v>
       </c>
@@ -8647,7 +8646,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="118" spans="1:20" hidden="1">
+    <row r="118" spans="1:20">
       <c r="A118" s="1" t="s">
         <v>145</v>
       </c>
@@ -8709,7 +8708,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="119" spans="1:20" hidden="1">
+    <row r="119" spans="1:20">
       <c r="A119" s="1" t="s">
         <v>145</v>
       </c>
@@ -8771,7 +8770,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="120" spans="1:20" hidden="1">
+    <row r="120" spans="1:20">
       <c r="A120" s="1" t="s">
         <v>145</v>
       </c>
@@ -8895,7 +8894,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="122" spans="1:20" hidden="1">
+    <row r="122" spans="1:20">
       <c r="A122" s="1">
         <v>94</v>
       </c>
@@ -8957,7 +8956,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="123" spans="1:20" hidden="1">
+    <row r="123" spans="1:20">
       <c r="A123" s="1" t="s">
         <v>149</v>
       </c>
@@ -9019,7 +9018,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="124" spans="1:20" hidden="1">
+    <row r="124" spans="1:20">
       <c r="A124" s="1">
         <v>94</v>
       </c>
@@ -9081,7 +9080,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="125" spans="1:20" hidden="1">
+    <row r="125" spans="1:20">
       <c r="A125" s="1">
         <v>94</v>
       </c>
@@ -9143,7 +9142,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="126" spans="1:20" hidden="1">
+    <row r="126" spans="1:20">
       <c r="A126" s="1">
         <v>94</v>
       </c>
@@ -9205,7 +9204,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="127" spans="1:20" hidden="1">
+    <row r="127" spans="1:20">
       <c r="A127" s="1" t="s">
         <v>149</v>
       </c>
@@ -9267,7 +9266,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="128" spans="1:20" hidden="1">
+    <row r="128" spans="1:20">
       <c r="A128" s="1" t="s">
         <v>145</v>
       </c>
@@ -9329,7 +9328,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="129" spans="1:20" hidden="1">
+    <row r="129" spans="1:20">
       <c r="A129" s="1" t="s">
         <v>149</v>
       </c>
@@ -9391,7 +9390,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="130" spans="1:20" hidden="1">
+    <row r="130" spans="1:20">
       <c r="A130" s="1" t="s">
         <v>149</v>
       </c>
@@ -9577,7 +9576,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="133" spans="1:20" hidden="1">
+    <row r="133" spans="1:20">
       <c r="A133" s="1">
         <v>94</v>
       </c>
@@ -9825,7 +9824,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="137" spans="1:20" hidden="1">
+    <row r="137" spans="1:20">
       <c r="A137" s="1" t="s">
         <v>147</v>
       </c>
@@ -9887,7 +9886,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="138" spans="1:20" hidden="1">
+    <row r="138" spans="1:20">
       <c r="A138" s="1" t="s">
         <v>145</v>
       </c>
@@ -10011,7 +10010,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="140" spans="1:20" hidden="1">
+    <row r="140" spans="1:20">
       <c r="A140" s="1">
         <v>94</v>
       </c>
@@ -10135,7 +10134,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="142" spans="1:20" hidden="1">
+    <row r="142" spans="1:20">
       <c r="A142" s="1">
         <v>94</v>
       </c>
@@ -10197,7 +10196,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="143" spans="1:20" hidden="1">
+    <row r="143" spans="1:20">
       <c r="A143" s="1" t="s">
         <v>145</v>
       </c>
@@ -10259,7 +10258,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="144" spans="1:20" hidden="1">
+    <row r="144" spans="1:20">
       <c r="A144" s="1" t="s">
         <v>145</v>
       </c>
@@ -10383,7 +10382,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="146" spans="1:20" hidden="1">
+    <row r="146" spans="1:20">
       <c r="A146" s="1">
         <v>94</v>
       </c>
@@ -10445,7 +10444,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="147" spans="1:20" hidden="1">
+    <row r="147" spans="1:20">
       <c r="A147" s="1" t="s">
         <v>145</v>
       </c>
@@ -10507,7 +10506,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="148" spans="1:20" hidden="1">
+    <row r="148" spans="1:20">
       <c r="A148" s="1" t="s">
         <v>145</v>
       </c>
@@ -10569,7 +10568,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="149" spans="1:20" hidden="1">
+    <row r="149" spans="1:20">
       <c r="A149" s="1">
         <v>94</v>
       </c>
@@ -10631,7 +10630,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="150" spans="1:20" hidden="1">
+    <row r="150" spans="1:20">
       <c r="A150" s="1">
         <v>94</v>
       </c>
@@ -10693,7 +10692,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="151" spans="1:20" hidden="1">
+    <row r="151" spans="1:20">
       <c r="A151" s="1">
         <v>94</v>
       </c>
@@ -10755,7 +10754,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="152" spans="1:20" hidden="1">
+    <row r="152" spans="1:20">
       <c r="A152" s="1">
         <v>94</v>
       </c>
@@ -11003,7 +11002,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="156" spans="1:20" hidden="1">
+    <row r="156" spans="1:20">
       <c r="A156" s="1" t="s">
         <v>147</v>
       </c>
@@ -11065,7 +11064,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="157" spans="1:20" hidden="1">
+    <row r="157" spans="1:20">
       <c r="A157" s="1" t="s">
         <v>147</v>
       </c>
@@ -11127,7 +11126,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="158" spans="1:20" hidden="1">
+    <row r="158" spans="1:20">
       <c r="A158" s="1" t="s">
         <v>147</v>
       </c>
@@ -11313,7 +11312,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="161" spans="1:20" hidden="1">
+    <row r="161" spans="1:20">
       <c r="A161" s="1">
         <v>94</v>
       </c>
@@ -11375,7 +11374,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="162" spans="1:20" hidden="1">
+    <row r="162" spans="1:20">
       <c r="A162" s="1">
         <v>94</v>
       </c>
@@ -11437,7 +11436,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="163" spans="1:20" hidden="1">
+    <row r="163" spans="1:20">
       <c r="A163" s="1">
         <v>94</v>
       </c>
@@ -11499,7 +11498,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="164" spans="1:20" hidden="1">
+    <row r="164" spans="1:20">
       <c r="A164" s="1">
         <v>94</v>
       </c>
@@ -11561,7 +11560,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="165" spans="1:20" hidden="1">
+    <row r="165" spans="1:20">
       <c r="A165" s="1">
         <v>94</v>
       </c>
@@ -11623,7 +11622,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="166" spans="1:20" hidden="1">
+    <row r="166" spans="1:20">
       <c r="A166" s="1" t="s">
         <v>145</v>
       </c>
@@ -11685,7 +11684,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="167" spans="1:20" hidden="1">
+    <row r="167" spans="1:20">
       <c r="A167" s="1" t="s">
         <v>145</v>
       </c>
@@ -11747,7 +11746,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="168" spans="1:20" hidden="1">
+    <row r="168" spans="1:20">
       <c r="A168" s="1" t="s">
         <v>145</v>
       </c>
@@ -11809,7 +11808,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="169" spans="1:20" hidden="1">
+    <row r="169" spans="1:20">
       <c r="A169" s="1" t="s">
         <v>145</v>
       </c>
@@ -11871,7 +11870,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="170" spans="1:20" hidden="1">
+    <row r="170" spans="1:20">
       <c r="A170" s="1" t="s">
         <v>145</v>
       </c>
@@ -11933,7 +11932,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="171" spans="1:20" hidden="1">
+    <row r="171" spans="1:20">
       <c r="A171" s="1" t="s">
         <v>145</v>
       </c>
@@ -12119,7 +12118,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="174" spans="1:20" hidden="1">
+    <row r="174" spans="1:20">
       <c r="A174" s="1" t="s">
         <v>147</v>
       </c>
@@ -12181,7 +12180,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="175" spans="1:20" hidden="1">
+    <row r="175" spans="1:20">
       <c r="A175" s="1" t="s">
         <v>147</v>
       </c>
@@ -12429,7 +12428,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="179" spans="1:20" hidden="1">
+    <row r="179" spans="1:20">
       <c r="A179" s="1" t="s">
         <v>145</v>
       </c>
@@ -12491,7 +12490,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="180" spans="1:20" hidden="1">
+    <row r="180" spans="1:20">
       <c r="A180" s="1" t="s">
         <v>145</v>
       </c>
@@ -12553,7 +12552,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="181" spans="1:20" hidden="1">
+    <row r="181" spans="1:20">
       <c r="A181" s="1" t="s">
         <v>145</v>
       </c>
@@ -12615,7 +12614,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="182" spans="1:20" hidden="1">
+    <row r="182" spans="1:20">
       <c r="A182" s="1" t="s">
         <v>145</v>
       </c>
@@ -12677,7 +12676,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="183" spans="1:20" hidden="1">
+    <row r="183" spans="1:20">
       <c r="A183" s="1">
         <v>94</v>
       </c>
@@ -12801,7 +12800,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="185" spans="1:20" hidden="1">
+    <row r="185" spans="1:20">
       <c r="A185" s="1">
         <v>94</v>
       </c>
@@ -12863,7 +12862,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="186" spans="1:20" hidden="1">
+    <row r="186" spans="1:20">
       <c r="A186" s="1">
         <v>94</v>
       </c>
@@ -12925,7 +12924,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="187" spans="1:20" hidden="1">
+    <row r="187" spans="1:20">
       <c r="A187" s="1" t="s">
         <v>145</v>
       </c>
@@ -12987,7 +12986,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="188" spans="1:20" hidden="1">
+    <row r="188" spans="1:20">
       <c r="A188" s="1">
         <v>94</v>
       </c>
@@ -13111,7 +13110,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="190" spans="1:20" hidden="1">
+    <row r="190" spans="1:20">
       <c r="A190" s="1">
         <v>15</v>
       </c>
@@ -13173,7 +13172,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="191" spans="1:20" hidden="1">
+    <row r="191" spans="1:20">
       <c r="A191" s="1">
         <v>15</v>
       </c>
@@ -13235,7 +13234,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="192" spans="1:20" hidden="1">
+    <row r="192" spans="1:20">
       <c r="A192" s="1">
         <v>15</v>
       </c>
@@ -13297,7 +13296,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="193" spans="1:20" hidden="1">
+    <row r="193" spans="1:20">
       <c r="A193" s="1">
         <v>15</v>
       </c>
@@ -13359,7 +13358,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="194" spans="1:20" hidden="1">
+    <row r="194" spans="1:20">
       <c r="A194" s="1">
         <v>15</v>
       </c>
@@ -13421,7 +13420,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="195" spans="1:20" hidden="1">
+    <row r="195" spans="1:20">
       <c r="A195" s="1" t="s">
         <v>19</v>
       </c>
@@ -13483,7 +13482,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="196" spans="1:20" hidden="1">
+    <row r="196" spans="1:20">
       <c r="A196" s="1" t="s">
         <v>39</v>
       </c>
@@ -13545,7 +13544,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="197" spans="1:20" hidden="1">
+    <row r="197" spans="1:20">
       <c r="A197" s="1" t="s">
         <v>22</v>
       </c>
@@ -13607,7 +13606,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="198" spans="1:20" hidden="1">
+    <row r="198" spans="1:20">
       <c r="A198" s="1" t="s">
         <v>19</v>
       </c>
@@ -13669,7 +13668,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="199" spans="1:20" ht="14.25" hidden="1" customHeight="1">
+    <row r="199" spans="1:20" ht="14.25" customHeight="1">
       <c r="A199" s="1" t="s">
         <v>19</v>
       </c>
@@ -13731,7 +13730,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="200" spans="1:20" hidden="1">
+    <row r="200" spans="1:20">
       <c r="A200" s="1" t="s">
         <v>19</v>
       </c>
@@ -13793,7 +13792,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="201" spans="1:20" hidden="1">
+    <row r="201" spans="1:20">
       <c r="A201" s="1" t="s">
         <v>19</v>
       </c>
@@ -13855,7 +13854,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="202" spans="1:20" hidden="1">
+    <row r="202" spans="1:20">
       <c r="A202" s="1" t="s">
         <v>22</v>
       </c>
@@ -13917,7 +13916,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="203" spans="1:20" hidden="1">
+    <row r="203" spans="1:20">
       <c r="A203" s="1" t="s">
         <v>22</v>
       </c>
@@ -13979,7 +13978,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="204" spans="1:20" hidden="1">
+    <row r="204" spans="1:20">
       <c r="A204" s="1" t="s">
         <v>22</v>
       </c>
@@ -14041,7 +14040,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="205" spans="1:20" hidden="1">
+    <row r="205" spans="1:20">
       <c r="A205" s="1" t="s">
         <v>22</v>
       </c>
@@ -14103,7 +14102,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="206" spans="1:20" hidden="1">
+    <row r="206" spans="1:20">
       <c r="A206" s="1" t="s">
         <v>19</v>
       </c>
@@ -14165,7 +14164,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="207" spans="1:20" hidden="1">
+    <row r="207" spans="1:20">
       <c r="A207" s="1" t="s">
         <v>19</v>
       </c>
@@ -14227,7 +14226,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="208" spans="1:20" hidden="1">
+    <row r="208" spans="1:20">
       <c r="A208" s="1" t="s">
         <v>19</v>
       </c>
@@ -14289,7 +14288,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="209" spans="1:20" hidden="1">
+    <row r="209" spans="1:20">
       <c r="A209" s="1" t="s">
         <v>19</v>
       </c>
@@ -14351,7 +14350,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="210" spans="1:20" hidden="1">
+    <row r="210" spans="1:20">
       <c r="A210" s="1" t="s">
         <v>19</v>
       </c>
@@ -14413,7 +14412,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="211" spans="1:20" hidden="1">
+    <row r="211" spans="1:20">
       <c r="A211" s="1" t="s">
         <v>18</v>
       </c>
@@ -14475,7 +14474,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="212" spans="1:20" hidden="1">
+    <row r="212" spans="1:20">
       <c r="A212" s="1" t="s">
         <v>18</v>
       </c>
@@ -14537,7 +14536,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="213" spans="1:20" hidden="1">
+    <row r="213" spans="1:20">
       <c r="A213" s="1" t="s">
         <v>18</v>
       </c>
@@ -14599,7 +14598,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="214" spans="1:20" hidden="1">
+    <row r="214" spans="1:20">
       <c r="A214" s="1" t="s">
         <v>19</v>
       </c>
@@ -14661,7 +14660,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="215" spans="1:20" hidden="1">
+    <row r="215" spans="1:20">
       <c r="A215" s="1" t="s">
         <v>22</v>
       </c>
@@ -14723,7 +14722,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="216" spans="1:20" hidden="1">
+    <row r="216" spans="1:20">
       <c r="A216" s="1" t="s">
         <v>22</v>
       </c>
@@ -14785,7 +14784,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="217" spans="1:20" hidden="1">
+    <row r="217" spans="1:20">
       <c r="A217" s="1" t="s">
         <v>22</v>
       </c>
@@ -14847,7 +14846,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="218" spans="1:20" hidden="1">
+    <row r="218" spans="1:20">
       <c r="A218" s="1" t="s">
         <v>19</v>
       </c>
@@ -14909,7 +14908,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="219" spans="1:20" hidden="1">
+    <row r="219" spans="1:20">
       <c r="A219" s="1" t="s">
         <v>22</v>
       </c>
@@ -14971,7 +14970,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="220" spans="1:20" hidden="1">
+    <row r="220" spans="1:20">
       <c r="A220" s="1" t="s">
         <v>22</v>
       </c>
@@ -15033,7 +15032,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="221" spans="1:20" hidden="1">
+    <row r="221" spans="1:20">
       <c r="A221" s="1" t="s">
         <v>22</v>
       </c>
@@ -15095,7 +15094,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="222" spans="1:20" hidden="1">
+    <row r="222" spans="1:20">
       <c r="A222" s="1" t="s">
         <v>19</v>
       </c>
@@ -15157,7 +15156,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="223" spans="1:20" hidden="1">
+    <row r="223" spans="1:20">
       <c r="A223" s="1" t="s">
         <v>19</v>
       </c>
@@ -15219,7 +15218,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="224" spans="1:20" hidden="1">
+    <row r="224" spans="1:20">
       <c r="A224" s="1" t="s">
         <v>19</v>
       </c>
@@ -15281,7 +15280,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="225" spans="1:20" hidden="1">
+    <row r="225" spans="1:20">
       <c r="A225" s="1" t="s">
         <v>22</v>
       </c>
@@ -15343,7 +15342,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="226" spans="1:20" hidden="1">
+    <row r="226" spans="1:20">
       <c r="A226" s="1" t="s">
         <v>22</v>
       </c>
@@ -15405,7 +15404,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="227" spans="1:20" hidden="1">
+    <row r="227" spans="1:20">
       <c r="A227" s="1">
         <v>15</v>
       </c>
@@ -15467,7 +15466,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="228" spans="1:20" hidden="1">
+    <row r="228" spans="1:20">
       <c r="A228" s="1" t="s">
         <v>19</v>
       </c>
@@ -15529,7 +15528,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="229" spans="1:20" hidden="1">
+    <row r="229" spans="1:20">
       <c r="A229" s="1" t="s">
         <v>39</v>
       </c>
@@ -15591,7 +15590,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="230" spans="1:20" hidden="1">
+    <row r="230" spans="1:20">
       <c r="A230" s="1" t="s">
         <v>39</v>
       </c>
@@ -15653,7 +15652,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="231" spans="1:20" hidden="1">
+    <row r="231" spans="1:20">
       <c r="A231" s="1" t="s">
         <v>19</v>
       </c>
@@ -15715,7 +15714,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="232" spans="1:20" hidden="1">
+    <row r="232" spans="1:20">
       <c r="A232" s="1">
         <v>15</v>
       </c>
@@ -15777,7 +15776,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="233" spans="1:20" ht="32" hidden="1">
+    <row r="233" spans="1:20" ht="32">
       <c r="A233" s="1" t="s">
         <v>19</v>
       </c>
@@ -15839,7 +15838,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="234" spans="1:20" hidden="1">
+    <row r="234" spans="1:20">
       <c r="A234" s="1" t="s">
         <v>19</v>
       </c>
@@ -15901,7 +15900,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="235" spans="1:20" hidden="1">
+    <row r="235" spans="1:20">
       <c r="A235" s="1" t="s">
         <v>22</v>
       </c>
@@ -15963,7 +15962,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="236" spans="1:20" hidden="1">
+    <row r="236" spans="1:20">
       <c r="A236" s="1" t="s">
         <v>19</v>
       </c>
@@ -16025,7 +16024,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="237" spans="1:20" hidden="1">
+    <row r="237" spans="1:20">
       <c r="A237" s="1" t="s">
         <v>22</v>
       </c>
@@ -16087,7 +16086,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="238" spans="1:20" ht="32" hidden="1">
+    <row r="238" spans="1:20" ht="32">
       <c r="A238" s="1" t="s">
         <v>19</v>
       </c>
@@ -16149,7 +16148,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="239" spans="1:20" hidden="1">
+    <row r="239" spans="1:20">
       <c r="A239" s="1" t="s">
         <v>19</v>
       </c>
@@ -16211,7 +16210,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="240" spans="1:20" hidden="1">
+    <row r="240" spans="1:20">
       <c r="A240" s="1" t="s">
         <v>19</v>
       </c>
@@ -16273,7 +16272,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="241" spans="1:20" hidden="1">
+    <row r="241" spans="1:20">
       <c r="A241" s="1" t="s">
         <v>39</v>
       </c>
@@ -16335,7 +16334,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="242" spans="1:20" hidden="1">
+    <row r="242" spans="1:20">
       <c r="A242" s="1" t="s">
         <v>39</v>
       </c>
@@ -16397,7 +16396,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="243" spans="1:20" hidden="1">
+    <row r="243" spans="1:20">
       <c r="A243" s="1" t="s">
         <v>19</v>
       </c>
@@ -16459,7 +16458,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="244" spans="1:20" hidden="1">
+    <row r="244" spans="1:20">
       <c r="A244" s="1">
         <v>15</v>
       </c>
@@ -16521,7 +16520,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="245" spans="1:20" hidden="1">
+    <row r="245" spans="1:20">
       <c r="A245" s="1" t="s">
         <v>39</v>
       </c>
@@ -16583,7 +16582,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="246" spans="1:20" hidden="1">
+    <row r="246" spans="1:20">
       <c r="A246" s="1" t="s">
         <v>39</v>
       </c>
@@ -16645,7 +16644,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="247" spans="1:20" hidden="1">
+    <row r="247" spans="1:20">
       <c r="A247" s="1" t="s">
         <v>39</v>
       </c>
@@ -16707,7 +16706,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="248" spans="1:20" hidden="1">
+    <row r="248" spans="1:20">
       <c r="A248" s="1" t="s">
         <v>22</v>
       </c>
@@ -16769,7 +16768,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="249" spans="1:20" hidden="1">
+    <row r="249" spans="1:20">
       <c r="A249" s="1" t="s">
         <v>22</v>
       </c>
@@ -16831,7 +16830,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="250" spans="1:20" hidden="1">
+    <row r="250" spans="1:20">
       <c r="A250" s="1">
         <v>15</v>
       </c>
@@ -16893,7 +16892,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="251" spans="1:20" hidden="1">
+    <row r="251" spans="1:20">
       <c r="A251" s="1">
         <v>15</v>
       </c>
@@ -16955,7 +16954,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="252" spans="1:20" hidden="1">
+    <row r="252" spans="1:20">
       <c r="A252" s="1" t="s">
         <v>39</v>
       </c>
@@ -17017,7 +17016,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="253" spans="1:20" hidden="1">
+    <row r="253" spans="1:20">
       <c r="A253" s="1" t="s">
         <v>39</v>
       </c>
@@ -17079,7 +17078,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="254" spans="1:20" hidden="1">
+    <row r="254" spans="1:20">
       <c r="A254" s="1" t="s">
         <v>19</v>
       </c>
@@ -17141,7 +17140,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="255" spans="1:20" hidden="1">
+    <row r="255" spans="1:20">
       <c r="A255" s="1" t="s">
         <v>19</v>
       </c>
@@ -17203,7 +17202,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="256" spans="1:20" hidden="1">
+    <row r="256" spans="1:20">
       <c r="A256" s="1" t="s">
         <v>39</v>
       </c>
@@ -17265,7 +17264,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="257" spans="1:20" hidden="1">
+    <row r="257" spans="1:20">
       <c r="A257" s="1">
         <v>15</v>
       </c>
@@ -17327,7 +17326,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="258" spans="1:20" hidden="1">
+    <row r="258" spans="1:20">
       <c r="A258" s="1">
         <v>15</v>
       </c>
@@ -17389,7 +17388,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="259" spans="1:20" hidden="1">
+    <row r="259" spans="1:20">
       <c r="A259" s="1">
         <v>15</v>
       </c>
@@ -17451,7 +17450,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="260" spans="1:20" hidden="1">
+    <row r="260" spans="1:20">
       <c r="A260" s="1" t="s">
         <v>39</v>
       </c>
@@ -17513,7 +17512,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="261" spans="1:20" hidden="1">
+    <row r="261" spans="1:20">
       <c r="A261" s="1">
         <v>15</v>
       </c>
@@ -17575,7 +17574,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="262" spans="1:20" hidden="1">
+    <row r="262" spans="1:20">
       <c r="A262" s="1">
         <v>15</v>
       </c>
@@ -17637,7 +17636,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="263" spans="1:20" hidden="1">
+    <row r="263" spans="1:20">
       <c r="A263" s="1" t="s">
         <v>39</v>
       </c>
@@ -17699,7 +17698,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="264" spans="1:20" hidden="1">
+    <row r="264" spans="1:20">
       <c r="A264" s="1">
         <v>15</v>
       </c>
@@ -17761,7 +17760,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="265" spans="1:20" hidden="1">
+    <row r="265" spans="1:20">
       <c r="A265" s="1">
         <v>15</v>
       </c>
@@ -17823,7 +17822,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="266" spans="1:20" hidden="1">
+    <row r="266" spans="1:20">
       <c r="A266" s="1" t="s">
         <v>39</v>
       </c>
@@ -17885,7 +17884,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="267" spans="1:20" hidden="1">
+    <row r="267" spans="1:20">
       <c r="A267" s="1">
         <v>15</v>
       </c>
@@ -17947,7 +17946,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="268" spans="1:20" hidden="1">
+    <row r="268" spans="1:20">
       <c r="A268" s="1" t="s">
         <v>39</v>
       </c>
@@ -18009,7 +18008,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="269" spans="1:20" hidden="1">
+    <row r="269" spans="1:20">
       <c r="A269" s="1">
         <v>15</v>
       </c>
@@ -18071,7 +18070,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="270" spans="1:20" hidden="1">
+    <row r="270" spans="1:20">
       <c r="A270" s="1">
         <v>15</v>
       </c>
@@ -18133,7 +18132,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="271" spans="1:20" hidden="1">
+    <row r="271" spans="1:20">
       <c r="A271" s="1">
         <v>15</v>
       </c>
@@ -18195,7 +18194,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="272" spans="1:20" hidden="1">
+    <row r="272" spans="1:20">
       <c r="A272" s="1">
         <v>15</v>
       </c>
@@ -18257,7 +18256,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="273" spans="1:20" hidden="1">
+    <row r="273" spans="1:20">
       <c r="A273" s="1">
         <v>15</v>
       </c>
@@ -18319,7 +18318,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="274" spans="1:20" hidden="1">
+    <row r="274" spans="1:20">
       <c r="A274" s="1">
         <v>15</v>
       </c>
@@ -18381,7 +18380,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="275" spans="1:20" hidden="1">
+    <row r="275" spans="1:20">
       <c r="A275" s="1" t="s">
         <v>39</v>
       </c>
@@ -18443,7 +18442,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="276" spans="1:20" hidden="1">
+    <row r="276" spans="1:20">
       <c r="A276" s="1" t="s">
         <v>39</v>
       </c>
@@ -18505,7 +18504,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="277" spans="1:20" hidden="1">
+    <row r="277" spans="1:20">
       <c r="A277" s="1" t="s">
         <v>39</v>
       </c>
@@ -18567,7 +18566,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="278" spans="1:20" hidden="1">
+    <row r="278" spans="1:20">
       <c r="A278" s="1">
         <v>15</v>
       </c>
@@ -18629,7 +18628,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="279" spans="1:20" hidden="1">
+    <row r="279" spans="1:20">
       <c r="A279" s="1">
         <v>15</v>
       </c>
@@ -18691,7 +18690,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="280" spans="1:20" hidden="1">
+    <row r="280" spans="1:20">
       <c r="A280" s="1">
         <v>15</v>
       </c>
@@ -18753,7 +18752,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="281" spans="1:20" hidden="1">
+    <row r="281" spans="1:20">
       <c r="A281" s="1">
         <v>15</v>
       </c>
@@ -18815,7 +18814,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="282" spans="1:20" hidden="1">
+    <row r="282" spans="1:20">
       <c r="A282" s="1">
         <v>15</v>
       </c>
@@ -18877,7 +18876,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="283" spans="1:20" hidden="1">
+    <row r="283" spans="1:20">
       <c r="A283" s="1">
         <v>15</v>
       </c>
@@ -18939,7 +18938,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="284" spans="1:20" hidden="1">
+    <row r="284" spans="1:20">
       <c r="A284" s="1" t="s">
         <v>39</v>
       </c>
@@ -19001,7 +19000,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="285" spans="1:20" hidden="1">
+    <row r="285" spans="1:20">
       <c r="A285" s="1" t="s">
         <v>39</v>
       </c>
@@ -19063,7 +19062,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="286" spans="1:20" hidden="1">
+    <row r="286" spans="1:20">
       <c r="A286" s="1" t="s">
         <v>39</v>
       </c>
@@ -19125,7 +19124,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="287" spans="1:20" hidden="1">
+    <row r="287" spans="1:20">
       <c r="A287" s="1" t="s">
         <v>144</v>
       </c>
@@ -19187,7 +19186,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="288" spans="1:20" hidden="1">
+    <row r="288" spans="1:20">
       <c r="A288" s="1" t="s">
         <v>144</v>
       </c>
@@ -19249,7 +19248,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="289" spans="1:20" hidden="1">
+    <row r="289" spans="1:20">
       <c r="A289" s="1">
         <v>83</v>
       </c>
@@ -19311,7 +19310,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="290" spans="1:20" hidden="1">
+    <row r="290" spans="1:20">
       <c r="A290" s="1">
         <v>83</v>
       </c>
@@ -19373,7 +19372,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="291" spans="1:20" hidden="1">
+    <row r="291" spans="1:20">
       <c r="A291" s="1">
         <v>83</v>
       </c>
@@ -19435,7 +19434,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="292" spans="1:20" hidden="1">
+    <row r="292" spans="1:20">
       <c r="A292" s="1">
         <v>83</v>
       </c>
@@ -19497,7 +19496,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="293" spans="1:20" hidden="1">
+    <row r="293" spans="1:20">
       <c r="A293" s="1">
         <v>83</v>
       </c>
@@ -19559,7 +19558,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="294" spans="1:20" hidden="1">
+    <row r="294" spans="1:20">
       <c r="A294" s="1">
         <v>83</v>
       </c>
@@ -19621,7 +19620,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="295" spans="1:20" hidden="1">
+    <row r="295" spans="1:20">
       <c r="A295" s="1" t="s">
         <v>152</v>
       </c>
@@ -19683,7 +19682,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="296" spans="1:20" hidden="1">
+    <row r="296" spans="1:20">
       <c r="A296" s="1" t="s">
         <v>152</v>
       </c>
@@ -19745,7 +19744,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="297" spans="1:20" hidden="1">
+    <row r="297" spans="1:20">
       <c r="A297" s="1" t="s">
         <v>152</v>
       </c>
@@ -19807,7 +19806,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="298" spans="1:20" hidden="1">
+    <row r="298" spans="1:20">
       <c r="A298" s="1" t="s">
         <v>152</v>
       </c>
@@ -19869,7 +19868,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="299" spans="1:20" hidden="1">
+    <row r="299" spans="1:20">
       <c r="A299" s="1">
         <v>83</v>
       </c>
@@ -19931,7 +19930,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="300" spans="1:20" hidden="1">
+    <row r="300" spans="1:20">
       <c r="A300" s="1">
         <v>83</v>
       </c>
@@ -19993,7 +19992,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="301" spans="1:20" hidden="1">
+    <row r="301" spans="1:20">
       <c r="A301" s="1">
         <v>83</v>
       </c>
@@ -20055,7 +20054,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="302" spans="1:20" hidden="1">
+    <row r="302" spans="1:20">
       <c r="A302" s="1" t="s">
         <v>148</v>
       </c>
@@ -20117,7 +20116,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="303" spans="1:20" hidden="1">
+    <row r="303" spans="1:20">
       <c r="A303" s="1" t="s">
         <v>148</v>
       </c>
@@ -20179,7 +20178,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="304" spans="1:20" hidden="1">
+    <row r="304" spans="1:20">
       <c r="A304" s="1" t="s">
         <v>148</v>
       </c>
@@ -20241,7 +20240,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="305" spans="1:20" hidden="1">
+    <row r="305" spans="1:20">
       <c r="A305" s="1">
         <v>83</v>
       </c>
@@ -20303,7 +20302,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="306" spans="1:20" hidden="1">
+    <row r="306" spans="1:20">
       <c r="A306" s="1">
         <v>83</v>
       </c>
@@ -20365,7 +20364,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="307" spans="1:20" hidden="1">
+    <row r="307" spans="1:20">
       <c r="A307" s="1">
         <v>83</v>
       </c>
@@ -20427,7 +20426,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="308" spans="1:20" hidden="1">
+    <row r="308" spans="1:20">
       <c r="A308" s="1">
         <v>83</v>
       </c>
@@ -20489,7 +20488,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="309" spans="1:20" hidden="1">
+    <row r="309" spans="1:20">
       <c r="A309" s="1">
         <v>83</v>
       </c>
@@ -20551,7 +20550,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="310" spans="1:20" hidden="1">
+    <row r="310" spans="1:20">
       <c r="A310" s="1">
         <v>83</v>
       </c>
@@ -20613,7 +20612,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="311" spans="1:20" hidden="1">
+    <row r="311" spans="1:20">
       <c r="A311" s="1">
         <v>83</v>
       </c>
@@ -20675,7 +20674,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="312" spans="1:20" hidden="1">
+    <row r="312" spans="1:20">
       <c r="A312" s="1">
         <v>83</v>
       </c>
@@ -20737,7 +20736,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="313" spans="1:20" hidden="1">
+    <row r="313" spans="1:20">
       <c r="A313" s="1" t="s">
         <v>144</v>
       </c>
@@ -20799,7 +20798,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="314" spans="1:20" hidden="1">
+    <row r="314" spans="1:20">
       <c r="A314" s="1" t="s">
         <v>144</v>
       </c>
@@ -20861,7 +20860,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="315" spans="1:20" hidden="1">
+    <row r="315" spans="1:20">
       <c r="A315" s="1" t="s">
         <v>144</v>
       </c>
@@ -20923,7 +20922,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="316" spans="1:20" hidden="1">
+    <row r="316" spans="1:20">
       <c r="A316" s="1">
         <v>83</v>
       </c>
@@ -20985,7 +20984,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="317" spans="1:20" hidden="1">
+    <row r="317" spans="1:20">
       <c r="A317" s="1">
         <v>83</v>
       </c>
@@ -21047,7 +21046,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="318" spans="1:20" hidden="1">
+    <row r="318" spans="1:20">
       <c r="A318" s="1" t="s">
         <v>152</v>
       </c>
@@ -21109,7 +21108,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="319" spans="1:20" hidden="1">
+    <row r="319" spans="1:20">
       <c r="A319" s="1" t="s">
         <v>152</v>
       </c>
@@ -21171,7 +21170,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="320" spans="1:20" hidden="1">
+    <row r="320" spans="1:20">
       <c r="A320" s="1" t="s">
         <v>152</v>
       </c>
@@ -21233,7 +21232,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="321" spans="1:20" hidden="1">
+    <row r="321" spans="1:20">
       <c r="A321" s="1">
         <v>83</v>
       </c>
@@ -21295,7 +21294,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="322" spans="1:20" hidden="1">
+    <row r="322" spans="1:20">
       <c r="A322" s="1" t="s">
         <v>152</v>
       </c>
@@ -21357,7 +21356,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="323" spans="1:20" hidden="1">
+    <row r="323" spans="1:20">
       <c r="A323" s="1" t="s">
         <v>144</v>
       </c>
@@ -21419,7 +21418,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="324" spans="1:20" hidden="1">
+    <row r="324" spans="1:20">
       <c r="A324" s="1" t="s">
         <v>152</v>
       </c>
@@ -21481,7 +21480,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="325" spans="1:20" hidden="1">
+    <row r="325" spans="1:20">
       <c r="A325" s="1" t="s">
         <v>152</v>
       </c>
@@ -21543,7 +21542,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="326" spans="1:20" hidden="1">
+    <row r="326" spans="1:20">
       <c r="A326" s="1">
         <v>83</v>
       </c>
@@ -21605,7 +21604,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="327" spans="1:20" hidden="1">
+    <row r="327" spans="1:20">
       <c r="A327" s="1">
         <v>83</v>
       </c>
@@ -21667,7 +21666,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="328" spans="1:20" hidden="1">
+    <row r="328" spans="1:20">
       <c r="A328" s="1" t="s">
         <v>144</v>
       </c>
@@ -21729,7 +21728,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="329" spans="1:20" hidden="1">
+    <row r="329" spans="1:20">
       <c r="A329" s="1" t="s">
         <v>148</v>
       </c>
@@ -21791,7 +21790,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="330" spans="1:20" hidden="1">
+    <row r="330" spans="1:20">
       <c r="A330" s="1" t="s">
         <v>148</v>
       </c>
@@ -21853,7 +21852,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="331" spans="1:20" hidden="1">
+    <row r="331" spans="1:20">
       <c r="A331" s="1" t="s">
         <v>148</v>
       </c>
@@ -21915,7 +21914,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="332" spans="1:20" hidden="1">
+    <row r="332" spans="1:20">
       <c r="A332" s="1" t="s">
         <v>148</v>
       </c>
@@ -21977,7 +21976,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="333" spans="1:20" hidden="1">
+    <row r="333" spans="1:20">
       <c r="A333" s="1" t="s">
         <v>148</v>
       </c>
@@ -22039,7 +22038,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="334" spans="1:20" hidden="1">
+    <row r="334" spans="1:20">
       <c r="A334" s="1" t="s">
         <v>152</v>
       </c>
@@ -22101,7 +22100,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="335" spans="1:20" hidden="1">
+    <row r="335" spans="1:20">
       <c r="A335" s="1" t="s">
         <v>152</v>
       </c>
@@ -22163,7 +22162,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="336" spans="1:20" hidden="1">
+    <row r="336" spans="1:20">
       <c r="A336" s="1" t="s">
         <v>152</v>
       </c>
@@ -22225,7 +22224,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="337" spans="1:20" hidden="1">
+    <row r="337" spans="1:20">
       <c r="A337" s="1" t="s">
         <v>152</v>
       </c>
@@ -22287,7 +22286,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="338" spans="1:20" hidden="1">
+    <row r="338" spans="1:20">
       <c r="A338" s="1" t="s">
         <v>152</v>
       </c>
@@ -22349,7 +22348,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="339" spans="1:20" hidden="1">
+    <row r="339" spans="1:20">
       <c r="A339" s="1" t="s">
         <v>152</v>
       </c>
@@ -22411,7 +22410,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="340" spans="1:20" hidden="1">
+    <row r="340" spans="1:20">
       <c r="A340" s="1" t="s">
         <v>152</v>
       </c>
@@ -22473,7 +22472,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="341" spans="1:20" hidden="1">
+    <row r="341" spans="1:20">
       <c r="A341" s="1" t="s">
         <v>152</v>
       </c>
@@ -22535,7 +22534,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="342" spans="1:20" hidden="1">
+    <row r="342" spans="1:20">
       <c r="A342" s="1" t="s">
         <v>152</v>
       </c>
@@ -22597,7 +22596,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="343" spans="1:20" hidden="1">
+    <row r="343" spans="1:20">
       <c r="A343" s="1" t="s">
         <v>152</v>
       </c>
@@ -22659,7 +22658,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="344" spans="1:20" hidden="1">
+    <row r="344" spans="1:20">
       <c r="A344" s="1" t="s">
         <v>152</v>
       </c>
@@ -22721,7 +22720,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="345" spans="1:20" hidden="1">
+    <row r="345" spans="1:20">
       <c r="A345" s="1" t="s">
         <v>152</v>
       </c>
@@ -22783,7 +22782,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="346" spans="1:20" hidden="1">
+    <row r="346" spans="1:20">
       <c r="A346" s="1" t="s">
         <v>152</v>
       </c>
@@ -22845,7 +22844,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="347" spans="1:20" hidden="1">
+    <row r="347" spans="1:20">
       <c r="A347" s="1" t="s">
         <v>148</v>
       </c>
@@ -22907,7 +22906,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="348" spans="1:20" hidden="1">
+    <row r="348" spans="1:20">
       <c r="A348" s="1" t="s">
         <v>148</v>
       </c>
@@ -22969,7 +22968,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="349" spans="1:20" hidden="1">
+    <row r="349" spans="1:20">
       <c r="A349" s="1" t="s">
         <v>148</v>
       </c>
@@ -23031,7 +23030,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="350" spans="1:20" hidden="1">
+    <row r="350" spans="1:20">
       <c r="A350" s="1" t="s">
         <v>152</v>
       </c>
@@ -23093,7 +23092,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="351" spans="1:20" hidden="1">
+    <row r="351" spans="1:20">
       <c r="A351" s="1">
         <v>83</v>
       </c>
@@ -23155,7 +23154,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="352" spans="1:20" hidden="1">
+    <row r="352" spans="1:20">
       <c r="A352" s="1">
         <v>83</v>
       </c>
@@ -23217,7 +23216,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="353" spans="1:20" hidden="1">
+    <row r="353" spans="1:20">
       <c r="A353" s="1">
         <v>83</v>
       </c>
@@ -23279,7 +23278,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="354" spans="1:20" hidden="1">
+    <row r="354" spans="1:20">
       <c r="A354" s="1">
         <v>83</v>
       </c>
@@ -23341,7 +23340,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="355" spans="1:20" hidden="1">
+    <row r="355" spans="1:20">
       <c r="A355" s="1">
         <v>83</v>
       </c>
@@ -23403,7 +23402,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="356" spans="1:20" hidden="1">
+    <row r="356" spans="1:20">
       <c r="A356" s="1">
         <v>83</v>
       </c>
@@ -23465,7 +23464,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="357" spans="1:20" hidden="1">
+    <row r="357" spans="1:20">
       <c r="A357" s="1">
         <v>83</v>
       </c>
@@ -23527,7 +23526,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="358" spans="1:20" hidden="1">
+    <row r="358" spans="1:20">
       <c r="A358" s="1">
         <v>83</v>
       </c>
@@ -23589,7 +23588,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="359" spans="1:20" hidden="1">
+    <row r="359" spans="1:20">
       <c r="A359" s="1" t="s">
         <v>152</v>
       </c>
@@ -23651,560 +23650,57 @@
         <v>153</v>
       </c>
     </row>
-    <row r="360" spans="1:20" hidden="1"/>
-    <row r="361" spans="1:20" hidden="1"/>
-    <row r="362" spans="1:20" hidden="1"/>
-    <row r="363" spans="1:20" hidden="1"/>
-    <row r="364" spans="1:20" hidden="1"/>
-    <row r="365" spans="1:20" hidden="1"/>
-    <row r="366" spans="1:20" hidden="1"/>
-    <row r="367" spans="1:20" hidden="1">
+    <row r="367" spans="1:20">
       <c r="E367" s="7"/>
     </row>
-    <row r="368" spans="1:20" hidden="1"/>
-    <row r="369" spans="5:5" hidden="1">
+    <row r="369" spans="5:5">
       <c r="E369" s="7"/>
     </row>
-    <row r="370" spans="5:5" hidden="1"/>
-    <row r="371" spans="5:5" hidden="1"/>
-    <row r="372" spans="5:5" hidden="1"/>
-    <row r="373" spans="5:5" hidden="1"/>
-    <row r="374" spans="5:5" hidden="1"/>
-    <row r="375" spans="5:5" hidden="1"/>
-    <row r="376" spans="5:5" hidden="1"/>
-    <row r="377" spans="5:5" hidden="1"/>
-    <row r="378" spans="5:5" hidden="1"/>
-    <row r="379" spans="5:5" hidden="1"/>
-    <row r="380" spans="5:5" hidden="1"/>
-    <row r="381" spans="5:5" hidden="1"/>
-    <row r="382" spans="5:5" hidden="1"/>
-    <row r="383" spans="5:5" hidden="1"/>
-    <row r="384" spans="5:5" hidden="1"/>
-    <row r="385" hidden="1"/>
-    <row r="386" hidden="1"/>
-    <row r="387" hidden="1"/>
-    <row r="388" hidden="1"/>
-    <row r="389" hidden="1"/>
-    <row r="390" hidden="1"/>
-    <row r="391" hidden="1"/>
-    <row r="392" hidden="1"/>
-    <row r="393" hidden="1"/>
-    <row r="394" hidden="1"/>
-    <row r="395" hidden="1"/>
-    <row r="396" hidden="1"/>
-    <row r="397" hidden="1"/>
-    <row r="398" hidden="1"/>
-    <row r="399" hidden="1"/>
-    <row r="400" hidden="1"/>
-    <row r="401" spans="16:16" hidden="1"/>
-    <row r="402" spans="16:16" hidden="1"/>
-    <row r="403" spans="16:16" hidden="1"/>
-    <row r="404" spans="16:16" hidden="1"/>
-    <row r="405" spans="16:16" hidden="1"/>
-    <row r="406" spans="16:16" hidden="1"/>
-    <row r="407" spans="16:16" hidden="1"/>
-    <row r="408" spans="16:16" hidden="1"/>
-    <row r="409" spans="16:16" hidden="1"/>
-    <row r="410" spans="16:16" hidden="1"/>
-    <row r="411" spans="16:16" hidden="1">
+    <row r="411" spans="16:16">
       <c r="P411" s="2"/>
     </row>
-    <row r="412" spans="16:16" hidden="1"/>
-    <row r="413" spans="16:16" hidden="1"/>
-    <row r="414" spans="16:16" hidden="1"/>
-    <row r="415" spans="16:16" hidden="1"/>
-    <row r="416" spans="16:16" hidden="1"/>
-    <row r="417" hidden="1"/>
-    <row r="418" hidden="1"/>
-    <row r="419" hidden="1"/>
-    <row r="420" hidden="1"/>
-    <row r="421" hidden="1"/>
-    <row r="422" hidden="1"/>
-    <row r="423" hidden="1"/>
-    <row r="424" hidden="1"/>
-    <row r="425" hidden="1"/>
-    <row r="426" hidden="1"/>
-    <row r="427" hidden="1"/>
-    <row r="428" hidden="1"/>
-    <row r="429" hidden="1"/>
-    <row r="430" hidden="1"/>
-    <row r="431" hidden="1"/>
-    <row r="432" hidden="1"/>
-    <row r="433" hidden="1"/>
-    <row r="434" hidden="1"/>
-    <row r="435" hidden="1"/>
-    <row r="436" hidden="1"/>
-    <row r="437" hidden="1"/>
-    <row r="438" hidden="1"/>
-    <row r="439" hidden="1"/>
-    <row r="440" hidden="1"/>
-    <row r="441" hidden="1"/>
-    <row r="442" hidden="1"/>
-    <row r="443" hidden="1"/>
-    <row r="444" hidden="1"/>
-    <row r="445" hidden="1"/>
-    <row r="446" hidden="1"/>
-    <row r="447" hidden="1"/>
-    <row r="448" hidden="1"/>
-    <row r="449" spans="16:16" hidden="1"/>
-    <row r="450" spans="16:16" hidden="1">
+    <row r="450" spans="16:16">
       <c r="P450" s="2"/>
     </row>
-    <row r="451" spans="16:16" hidden="1">
+    <row r="451" spans="16:16">
       <c r="P451" s="2"/>
     </row>
-    <row r="452" spans="16:16" hidden="1">
+    <row r="452" spans="16:16">
       <c r="P452" s="2"/>
     </row>
-    <row r="453" spans="16:16" hidden="1">
+    <row r="453" spans="16:16">
       <c r="P453" s="2"/>
     </row>
-    <row r="454" spans="16:16" hidden="1"/>
-    <row r="455" spans="16:16" hidden="1"/>
-    <row r="456" spans="16:16" hidden="1"/>
-    <row r="457" spans="16:16" hidden="1"/>
-    <row r="458" spans="16:16" hidden="1"/>
-    <row r="459" spans="16:16" hidden="1"/>
-    <row r="460" spans="16:16" hidden="1"/>
-    <row r="461" spans="16:16" hidden="1"/>
-    <row r="462" spans="16:16" hidden="1"/>
-    <row r="463" spans="16:16" hidden="1"/>
-    <row r="464" spans="16:16" hidden="1"/>
-    <row r="465" spans="16:16" hidden="1"/>
-    <row r="466" spans="16:16" hidden="1"/>
-    <row r="467" spans="16:16" hidden="1"/>
-    <row r="468" spans="16:16" hidden="1">
+    <row r="468" spans="16:16">
       <c r="P468" s="2"/>
     </row>
-    <row r="469" spans="16:16" hidden="1"/>
-    <row r="470" spans="16:16" hidden="1"/>
-    <row r="471" spans="16:16" hidden="1"/>
-    <row r="472" spans="16:16" hidden="1"/>
-    <row r="473" spans="16:16" hidden="1"/>
-    <row r="474" spans="16:16" hidden="1"/>
-    <row r="475" spans="16:16" hidden="1"/>
-    <row r="476" spans="16:16" hidden="1"/>
-    <row r="477" spans="16:16" hidden="1"/>
-    <row r="478" spans="16:16" hidden="1"/>
-    <row r="479" spans="16:16" hidden="1"/>
-    <row r="480" spans="16:16" hidden="1"/>
-    <row r="481" hidden="1"/>
-    <row r="482" hidden="1"/>
-    <row r="483" hidden="1"/>
-    <row r="484" hidden="1"/>
-    <row r="485" hidden="1"/>
-    <row r="486" hidden="1"/>
-    <row r="487" hidden="1"/>
-    <row r="488" hidden="1"/>
-    <row r="489" hidden="1"/>
-    <row r="490" hidden="1"/>
-    <row r="491" hidden="1"/>
-    <row r="492" hidden="1"/>
-    <row r="493" hidden="1"/>
-    <row r="494" hidden="1"/>
-    <row r="495" hidden="1"/>
-    <row r="496" hidden="1"/>
-    <row r="497" hidden="1"/>
-    <row r="498" hidden="1"/>
-    <row r="499" hidden="1"/>
-    <row r="500" hidden="1"/>
-    <row r="501" hidden="1"/>
-    <row r="502" hidden="1"/>
-    <row r="503" hidden="1"/>
-    <row r="504" hidden="1"/>
-    <row r="505" hidden="1"/>
-    <row r="506" hidden="1"/>
-    <row r="507" hidden="1"/>
-    <row r="508" hidden="1"/>
-    <row r="509" hidden="1"/>
-    <row r="510" hidden="1"/>
-    <row r="511" hidden="1"/>
-    <row r="512" hidden="1"/>
-    <row r="513" hidden="1"/>
-    <row r="514" hidden="1"/>
-    <row r="515" hidden="1"/>
-    <row r="516" hidden="1"/>
-    <row r="517" hidden="1"/>
-    <row r="518" hidden="1"/>
-    <row r="519" hidden="1"/>
-    <row r="520" hidden="1"/>
-    <row r="521" hidden="1"/>
-    <row r="522" hidden="1"/>
-    <row r="523" hidden="1"/>
-    <row r="524" hidden="1"/>
-    <row r="525" hidden="1"/>
-    <row r="526" hidden="1"/>
-    <row r="527" hidden="1"/>
-    <row r="528" hidden="1"/>
-    <row r="529" hidden="1"/>
-    <row r="530" hidden="1"/>
-    <row r="531" hidden="1"/>
-    <row r="532" hidden="1"/>
-    <row r="533" hidden="1"/>
-    <row r="534" hidden="1"/>
-    <row r="535" hidden="1"/>
-    <row r="536" hidden="1"/>
-    <row r="537" hidden="1"/>
-    <row r="538" hidden="1"/>
-    <row r="539" hidden="1"/>
-    <row r="540" hidden="1"/>
-    <row r="541" hidden="1"/>
-    <row r="542" hidden="1"/>
-    <row r="543" hidden="1"/>
-    <row r="544" hidden="1"/>
-    <row r="545" hidden="1"/>
-    <row r="546" hidden="1"/>
-    <row r="547" hidden="1"/>
-    <row r="548" hidden="1"/>
-    <row r="549" hidden="1"/>
-    <row r="550" hidden="1"/>
-    <row r="551" hidden="1"/>
-    <row r="552" hidden="1"/>
-    <row r="553" hidden="1"/>
-    <row r="554" hidden="1"/>
-    <row r="555" hidden="1"/>
-    <row r="556" hidden="1"/>
-    <row r="557" hidden="1"/>
-    <row r="558" hidden="1"/>
-    <row r="559" hidden="1"/>
-    <row r="560" hidden="1"/>
-    <row r="561" hidden="1"/>
-    <row r="562" hidden="1"/>
-    <row r="563" hidden="1"/>
-    <row r="564" hidden="1"/>
-    <row r="565" hidden="1"/>
-    <row r="566" hidden="1"/>
-    <row r="567" hidden="1"/>
-    <row r="568" hidden="1"/>
-    <row r="569" hidden="1"/>
-    <row r="570" hidden="1"/>
-    <row r="571" hidden="1"/>
-    <row r="572" hidden="1"/>
-    <row r="573" hidden="1"/>
-    <row r="574" hidden="1"/>
-    <row r="575" hidden="1"/>
-    <row r="576" hidden="1"/>
-    <row r="577" spans="16:16" hidden="1"/>
-    <row r="578" spans="16:16" hidden="1"/>
-    <row r="579" spans="16:16" hidden="1"/>
-    <row r="580" spans="16:16" hidden="1"/>
-    <row r="581" spans="16:16" hidden="1"/>
-    <row r="582" spans="16:16" hidden="1"/>
-    <row r="583" spans="16:16" hidden="1">
+    <row r="583" spans="16:16">
       <c r="P583" s="2"/>
     </row>
-    <row r="584" spans="16:16" hidden="1"/>
-    <row r="585" spans="16:16" hidden="1"/>
-    <row r="586" spans="16:16" hidden="1"/>
-    <row r="587" spans="16:16" hidden="1"/>
-    <row r="588" spans="16:16" hidden="1"/>
-    <row r="589" spans="16:16" hidden="1"/>
-    <row r="590" spans="16:16" hidden="1"/>
-    <row r="591" spans="16:16" hidden="1"/>
-    <row r="592" spans="16:16" hidden="1"/>
-    <row r="593" hidden="1"/>
-    <row r="594" hidden="1"/>
-    <row r="595" hidden="1"/>
-    <row r="596" hidden="1"/>
-    <row r="597" hidden="1"/>
-    <row r="598" hidden="1"/>
-    <row r="599" hidden="1"/>
-    <row r="600" hidden="1"/>
-    <row r="601" hidden="1"/>
-    <row r="602" hidden="1"/>
-    <row r="603" hidden="1"/>
-    <row r="604" hidden="1"/>
-    <row r="605" hidden="1"/>
-    <row r="606" hidden="1"/>
-    <row r="607" hidden="1"/>
-    <row r="608" hidden="1"/>
-    <row r="609" spans="16:16" hidden="1">
+    <row r="609" spans="16:16">
       <c r="P609" s="2"/>
     </row>
-    <row r="610" spans="16:16" hidden="1"/>
-    <row r="611" spans="16:16" hidden="1">
+    <row r="611" spans="16:16">
       <c r="P611" s="2"/>
     </row>
-    <row r="612" spans="16:16" hidden="1"/>
-    <row r="613" spans="16:16" hidden="1"/>
-    <row r="614" spans="16:16" hidden="1"/>
-    <row r="615" spans="16:16" hidden="1"/>
-    <row r="616" spans="16:16" hidden="1"/>
-    <row r="617" spans="16:16" hidden="1"/>
-    <row r="618" spans="16:16" hidden="1"/>
-    <row r="619" spans="16:16" hidden="1"/>
-    <row r="620" spans="16:16" hidden="1"/>
-    <row r="621" spans="16:16" hidden="1"/>
-    <row r="622" spans="16:16" hidden="1"/>
-    <row r="623" spans="16:16" hidden="1"/>
-    <row r="624" spans="16:16" hidden="1"/>
-    <row r="625" hidden="1"/>
-    <row r="626" hidden="1"/>
-    <row r="627" hidden="1"/>
-    <row r="628" hidden="1"/>
-    <row r="629" hidden="1"/>
-    <row r="630" hidden="1"/>
-    <row r="631" hidden="1"/>
-    <row r="632" hidden="1"/>
-    <row r="633" hidden="1"/>
-    <row r="634" hidden="1"/>
-    <row r="635" hidden="1"/>
-    <row r="636" hidden="1"/>
-    <row r="637" hidden="1"/>
-    <row r="638" hidden="1"/>
-    <row r="639" hidden="1"/>
-    <row r="640" hidden="1"/>
-    <row r="641" spans="16:16" hidden="1"/>
-    <row r="642" spans="16:16" hidden="1"/>
-    <row r="643" spans="16:16" hidden="1"/>
-    <row r="644" spans="16:16" hidden="1"/>
-    <row r="645" spans="16:16" hidden="1"/>
-    <row r="646" spans="16:16" hidden="1"/>
-    <row r="647" spans="16:16" hidden="1"/>
-    <row r="648" spans="16:16" hidden="1"/>
-    <row r="649" spans="16:16" hidden="1"/>
-    <row r="650" spans="16:16" hidden="1">
+    <row r="650" spans="16:16">
       <c r="P650" s="2"/>
     </row>
-    <row r="651" spans="16:16" hidden="1">
+    <row r="651" spans="16:16">
       <c r="P651" s="2"/>
     </row>
-    <row r="652" spans="16:16" hidden="1"/>
-    <row r="653" spans="16:16" hidden="1"/>
-    <row r="654" spans="16:16" hidden="1"/>
-    <row r="655" spans="16:16" hidden="1"/>
-    <row r="656" spans="16:16" hidden="1"/>
-    <row r="657" hidden="1"/>
-    <row r="658" hidden="1"/>
-    <row r="659" hidden="1"/>
-    <row r="660" hidden="1"/>
-    <row r="661" hidden="1"/>
-    <row r="662" hidden="1"/>
-    <row r="663" hidden="1"/>
-    <row r="664" hidden="1"/>
-    <row r="665" hidden="1"/>
-    <row r="666" hidden="1"/>
-    <row r="667" hidden="1"/>
-    <row r="668" hidden="1"/>
-    <row r="669" hidden="1"/>
-    <row r="670" hidden="1"/>
-    <row r="671" hidden="1"/>
-    <row r="672" hidden="1"/>
-    <row r="673" spans="16:16" hidden="1"/>
-    <row r="674" spans="16:16" hidden="1"/>
-    <row r="675" spans="16:16" hidden="1"/>
-    <row r="676" spans="16:16" hidden="1"/>
-    <row r="677" spans="16:16" hidden="1"/>
-    <row r="678" spans="16:16" hidden="1"/>
-    <row r="679" spans="16:16" hidden="1"/>
-    <row r="680" spans="16:16" hidden="1"/>
-    <row r="681" spans="16:16" hidden="1"/>
-    <row r="682" spans="16:16" hidden="1"/>
-    <row r="683" spans="16:16" hidden="1"/>
-    <row r="684" spans="16:16" hidden="1">
+    <row r="684" spans="16:16">
       <c r="P684" s="2"/>
     </row>
-    <row r="685" spans="16:16" hidden="1"/>
-    <row r="686" spans="16:16" hidden="1"/>
-    <row r="687" spans="16:16" hidden="1"/>
-    <row r="688" spans="16:16" hidden="1"/>
-    <row r="689" spans="16:16" hidden="1">
+    <row r="689" spans="16:16">
       <c r="P689" s="2"/>
     </row>
-    <row r="690" spans="16:16" hidden="1"/>
-    <row r="691" spans="16:16" hidden="1"/>
-    <row r="692" spans="16:16" hidden="1"/>
-    <row r="693" spans="16:16" hidden="1"/>
-    <row r="694" spans="16:16" hidden="1"/>
-    <row r="695" spans="16:16" hidden="1"/>
-    <row r="696" spans="16:16" hidden="1"/>
-    <row r="697" spans="16:16" hidden="1"/>
-    <row r="698" spans="16:16" hidden="1"/>
-    <row r="699" spans="16:16" hidden="1"/>
-    <row r="700" spans="16:16" hidden="1"/>
-    <row r="701" spans="16:16" hidden="1"/>
-    <row r="702" spans="16:16" hidden="1"/>
-    <row r="703" spans="16:16" hidden="1"/>
-    <row r="704" spans="16:16" hidden="1"/>
-    <row r="705" hidden="1"/>
-    <row r="706" hidden="1"/>
-    <row r="707" hidden="1"/>
-    <row r="708" hidden="1"/>
-    <row r="709" hidden="1"/>
-    <row r="710" hidden="1"/>
-    <row r="711" hidden="1"/>
-    <row r="712" hidden="1"/>
-    <row r="713" hidden="1"/>
-    <row r="714" hidden="1"/>
-    <row r="715" hidden="1"/>
-    <row r="716" hidden="1"/>
-    <row r="717" hidden="1"/>
-    <row r="718" hidden="1"/>
-    <row r="719" hidden="1"/>
-    <row r="720" hidden="1"/>
-    <row r="721" hidden="1"/>
-    <row r="722" hidden="1"/>
-    <row r="723" hidden="1"/>
-    <row r="724" hidden="1"/>
-    <row r="725" hidden="1"/>
-    <row r="726" hidden="1"/>
-    <row r="727" hidden="1"/>
-    <row r="728" hidden="1"/>
-    <row r="729" hidden="1"/>
-    <row r="730" hidden="1"/>
-    <row r="731" hidden="1"/>
-    <row r="732" hidden="1"/>
-    <row r="733" hidden="1"/>
-    <row r="734" hidden="1"/>
-    <row r="735" hidden="1"/>
-    <row r="736" hidden="1"/>
-    <row r="737" hidden="1"/>
-    <row r="738" hidden="1"/>
-    <row r="739" hidden="1"/>
-    <row r="740" hidden="1"/>
-    <row r="741" hidden="1"/>
-    <row r="742" hidden="1"/>
-    <row r="743" hidden="1"/>
-    <row r="744" hidden="1"/>
-    <row r="745" hidden="1"/>
-    <row r="746" hidden="1"/>
-    <row r="747" hidden="1"/>
-    <row r="748" hidden="1"/>
-    <row r="749" hidden="1"/>
-    <row r="750" hidden="1"/>
-    <row r="751" hidden="1"/>
-    <row r="752" hidden="1"/>
-    <row r="753" hidden="1"/>
-    <row r="754" hidden="1"/>
-    <row r="755" hidden="1"/>
-    <row r="756" hidden="1"/>
-    <row r="757" hidden="1"/>
-    <row r="758" hidden="1"/>
-    <row r="759" hidden="1"/>
-    <row r="760" hidden="1"/>
-    <row r="761" hidden="1"/>
-    <row r="762" hidden="1"/>
-    <row r="763" hidden="1"/>
-    <row r="764" hidden="1"/>
-    <row r="765" hidden="1"/>
-    <row r="766" hidden="1"/>
-    <row r="767" hidden="1"/>
-    <row r="768" hidden="1"/>
-    <row r="769" hidden="1"/>
-    <row r="770" hidden="1"/>
-    <row r="771" hidden="1"/>
-    <row r="772" hidden="1"/>
-    <row r="773" hidden="1"/>
-    <row r="774" hidden="1"/>
-    <row r="775" hidden="1"/>
-    <row r="776" hidden="1"/>
-    <row r="777" hidden="1"/>
-    <row r="778" hidden="1"/>
-    <row r="779" hidden="1"/>
-    <row r="780" hidden="1"/>
-    <row r="781" hidden="1"/>
-    <row r="782" hidden="1"/>
-    <row r="783" hidden="1"/>
-    <row r="784" hidden="1"/>
-    <row r="785" hidden="1"/>
-    <row r="786" hidden="1"/>
-    <row r="787" hidden="1"/>
-    <row r="788" hidden="1"/>
-    <row r="789" hidden="1"/>
-    <row r="790" hidden="1"/>
-    <row r="791" hidden="1"/>
-    <row r="792" hidden="1"/>
-    <row r="793" hidden="1"/>
-    <row r="794" hidden="1"/>
-    <row r="795" hidden="1"/>
-    <row r="796" hidden="1"/>
-    <row r="797" hidden="1"/>
-    <row r="798" hidden="1"/>
-    <row r="799" hidden="1"/>
-    <row r="800" hidden="1"/>
-    <row r="801" hidden="1"/>
-    <row r="802" hidden="1"/>
-    <row r="803" hidden="1"/>
-    <row r="804" hidden="1"/>
-    <row r="805" hidden="1"/>
-    <row r="806" hidden="1"/>
-    <row r="807" hidden="1"/>
-    <row r="808" hidden="1"/>
-    <row r="809" hidden="1"/>
-    <row r="810" hidden="1"/>
-    <row r="811" hidden="1"/>
-    <row r="812" hidden="1"/>
-    <row r="813" hidden="1"/>
-    <row r="814" hidden="1"/>
-    <row r="815" hidden="1"/>
-    <row r="816" hidden="1"/>
-    <row r="817" spans="16:16" hidden="1"/>
-    <row r="818" spans="16:16" hidden="1"/>
-    <row r="819" spans="16:16" hidden="1">
+    <row r="819" spans="16:16">
       <c r="P819" s="2"/>
     </row>
-    <row r="820" spans="16:16" hidden="1"/>
-    <row r="821" spans="16:16" hidden="1"/>
-    <row r="822" spans="16:16" hidden="1"/>
-    <row r="823" spans="16:16" hidden="1"/>
-    <row r="824" spans="16:16" hidden="1"/>
-    <row r="825" spans="16:16" hidden="1"/>
-    <row r="826" spans="16:16" hidden="1"/>
-    <row r="827" spans="16:16" hidden="1"/>
-    <row r="828" spans="16:16" hidden="1"/>
-    <row r="829" spans="16:16" hidden="1"/>
-    <row r="830" spans="16:16" hidden="1"/>
-    <row r="831" spans="16:16" hidden="1"/>
-    <row r="832" spans="16:16" hidden="1"/>
-    <row r="833" hidden="1"/>
-    <row r="834" hidden="1"/>
-    <row r="835" hidden="1"/>
-    <row r="836" hidden="1"/>
-    <row r="837" hidden="1"/>
-    <row r="838" hidden="1"/>
-    <row r="839" hidden="1"/>
-    <row r="840" hidden="1"/>
-    <row r="841" hidden="1"/>
-    <row r="842" hidden="1"/>
-    <row r="843" hidden="1"/>
-    <row r="844" hidden="1"/>
-    <row r="845" hidden="1"/>
-    <row r="846" hidden="1"/>
-    <row r="847" hidden="1"/>
-    <row r="848" hidden="1"/>
-    <row r="849" hidden="1"/>
-    <row r="850" hidden="1"/>
-    <row r="851" hidden="1"/>
-    <row r="852" hidden="1"/>
-    <row r="853" hidden="1"/>
-    <row r="854" hidden="1"/>
-    <row r="855" hidden="1"/>
-    <row r="856" hidden="1"/>
-    <row r="857" hidden="1"/>
-    <row r="858" hidden="1"/>
-    <row r="859" hidden="1"/>
-    <row r="860" hidden="1"/>
-    <row r="861" hidden="1"/>
-    <row r="862" hidden="1"/>
-    <row r="863" hidden="1"/>
-    <row r="864" hidden="1"/>
-    <row r="865" spans="16:16" hidden="1"/>
-    <row r="866" spans="16:16" hidden="1"/>
-    <row r="867" spans="16:16" hidden="1"/>
-    <row r="868" spans="16:16" hidden="1"/>
-    <row r="869" spans="16:16" hidden="1"/>
-    <row r="870" spans="16:16" hidden="1">
+    <row r="870" spans="16:16">
       <c r="P870" s="2"/>
     </row>
-    <row r="871" spans="16:16" hidden="1"/>
-    <row r="872" spans="16:16" hidden="1"/>
-    <row r="873" spans="16:16" hidden="1"/>
-    <row r="874" spans="16:16" hidden="1"/>
-    <row r="875" spans="16:16" hidden="1"/>
-    <row r="876" spans="16:16" hidden="1"/>
-    <row r="877" spans="16:16" hidden="1"/>
-    <row r="878" spans="16:16" hidden="1"/>
-    <row r="879" spans="16:16" hidden="1"/>
     <row r="882" spans="2:5">
       <c r="B882" s="4"/>
     </row>
@@ -24212,13 +23708,7 @@
       <c r="E885" s="5"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:A879" xr:uid="{00000000-0009-0000-0000-000000000000}">
-    <filterColumn colId="0">
-      <filters>
-        <filter val="7A"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:A879" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>

</xml_diff>